<commit_message>
some changes on the charts
</commit_message>
<xml_diff>
--- a/db/db_analysis/results/results.xlsx
+++ b/db/db_analysis/results/results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsghrg/workarea/work/zhaw_repos/s8/ba/releo/db/db_analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsghrg/workarea/work/zhaw_repos/s8/ba/releo/db/db_analysis/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759EB324-8F01-D54A-9C16-38F06F3C695F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF1AEA3-CFC6-D34F-90D0-3CF02982988B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="940" yWindow="500" windowWidth="67860" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21188,8 +21188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T685"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B67" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F83" sqref="F83:J84"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>